<commit_message>
Add cdnc & rsutaf in grib_table_126 branch by taking them off from the identified missing file for this branch #453
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables-enable-pextra.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables-enable-pextra.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="147">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -250,127 +250,82 @@
     <t xml:space="preserve">IfxAnt</t>
   </si>
   <si>
-    <t xml:space="preserve">AERmon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cdnc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">longitude latitude alevel time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cloud Liquid Droplet Number Concentration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">m-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">web</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grib 126.20 / 126.22        part of MFP3D        In namelist.ifs.cloudact+diag.sh  CVEXTRA(1)='CDNC' which is a PEXTRA variable.</t>
+    <t xml:space="preserve">Emon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intuadse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertically Integrated Eastward Dry Statice Energy Transport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MJ m-1 s-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in the standard IFS output. However, per layer the specific heat capacity of dry air (1005.7 J kg-1 K-1) can be multiplied by the Temperature (grib 128.130) times the V component of wind (grib 128.132) + the geopotential height  (grib 128.129) and this needs to be vertically integrated times the air density per layer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertically integrated eastward dry static energy transport (cp.T +zg).v (Mass_weighted_vertical integral of the product of eastward wind by dry static_energy per mass unit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intuaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertically Integrated Eastward Moisture Transport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kg m-1 s-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in the standard IFS output. However, per layer the Specific humidity (grib 128.133 + unit conversion) can be multiplied by the U component of wind (grib 128.131) and this needs to be vertically integrated.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertically integrated Eastward moisture transport (Mass weighted vertical integral of the product of eastward wind by total water mass per unit mass)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intvadse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertically Integrated Northward Dry Static Energy Transport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in the standard IFS output. However, per layer the specific heat capacity of dry air (1005.7 J kg-1 K-1) can be multiplied by the Temperature (grib 128.130) times the U component of wind (grib 128.131) + the geopotential height  (grib 128.129) and this needs to be vertically integrated times the air density per layer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertically integrated northward dry static energy transport (cp.T +zg).v (Mass_weighted_vertical integral of the product of northward wind by dry static_energy per mass unit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intvaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertically Integrated Northward Moisture Transport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in the standard IFS output. However, per layer the Specific humidity (grib 128.133 + unit conversion) can be multiplied by the V component of wind (grib 128.132) and this needs to be vertically integrated.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertically integrated Northward moisture transport (Mass_weighted_vertical integral of the product of northward wind by total water mass per unit mass)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">od550aerso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude time lambda550nm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stratospheric Optical Depth at 550nm (All Aerosols) 2D-Field (Stratosphere Only)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Determined by CMIP6 stratospheric aerosol forcing data set</t>
   </si>
   <si>
     <t xml:space="preserve">Twan &amp; Thomas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cloud Droplet Number Concentration in liquid water clouds.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AerChemMIP,CFMIP,DAMIP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rsutaf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">longitude latitude time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOA Outgoing Aerosol-Free Shortwave Radiation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">W m-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grib 128.212-126.069     part of MFPPHY    Available from double radiation call in IFS. PEXTRA issue #403   aerosol free</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flux corresponding to rsut resulting from aerosol-free call to radiation, following Ghan (ACP, 2013)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AerChemMIP,DAMIP,GeoMIP,HighResMIP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Emon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">intuadse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vertically Integrated Eastward Dry Statice Energy Transport</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MJ m-1 s-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not available in the standard IFS output. However, per layer the specific heat capacity of dry air (1005.7 J kg-1 K-1) can be multiplied by the Temperature (grib 128.130) times the V component of wind (grib 128.132) + the geopotential height  (grib 128.129) and this needs to be vertically integrated times the air density per layer.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vertically integrated eastward dry static energy transport (cp.T +zg).v (Mass_weighted_vertical integral of the product of eastward wind by dry static_energy per mass unit)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PMIP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">intuaw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vertically Integrated Eastward Moisture Transport</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kg m-1 s-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not available in the standard IFS output. However, per layer the Specific humidity (grib 128.133 + unit conversion) can be multiplied by the U component of wind (grib 128.131) and this needs to be vertically integrated.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vertically integrated Eastward moisture transport (Mass weighted vertical integral of the product of eastward wind by total water mass per unit mass)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">intvadse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vertically Integrated Northward Dry Static Energy Transport</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not available in the standard IFS output. However, per layer the specific heat capacity of dry air (1005.7 J kg-1 K-1) can be multiplied by the Temperature (grib 128.130) times the U component of wind (grib 128.131) + the geopotential height  (grib 128.129) and this needs to be vertically integrated times the air density per layer.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vertically integrated northward dry static energy transport (cp.T +zg).v (Mass_weighted_vertical integral of the product of northward wind by dry static_energy per mass unit)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">intvaw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vertically Integrated Northward Moisture Transport</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not available in the standard IFS output. However, per layer the Specific humidity (grib 128.133 + unit conversion) can be multiplied by the V component of wind (grib 128.132) and this needs to be vertically integrated.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vertically integrated Northward moisture transport (Mass_weighted_vertical integral of the product of northward wind by total water mass per unit mass)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">od550aerso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">longitude latitude time lambda550nm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stratospheric Optical Depth at 550nm (All Aerosols) 2D-Field (Stratosphere Only)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Determined by CMIP6 stratospheric aerosol forcing data set</t>
   </si>
   <si>
     <t xml:space="preserve">From tropopause to stratopause as defined by the model</t>
@@ -622,7 +577,7 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1131,20 +1086,21 @@
       <c r="F19" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="G19" s="0" t="s">
+      <c r="G19" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917acf0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="H19" s="0" t="s">
+      <c r="I19" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="J19" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="I19" s="0" t="s">
+      <c r="K19" s="0" t="s">
         <v>83</v>
-      </c>
-      <c r="J19" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="K19" s="0" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1152,129 +1108,166 @@
         <v>76</v>
       </c>
       <c r="B20" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="F20" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="C20" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="0" t="s">
+      <c r="G20" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590de58a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="I20" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="J20" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="F20" s="0" t="s">
+      <c r="K20" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="G20" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="H20" s="0" t="s">
+      <c r="C21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="I20" s="0" t="s">
+      <c r="F21" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59147b48-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="K21" s="0" t="s">
         <v>83</v>
-      </c>
-      <c r="J20" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="K20" s="0" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="C22" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="C22" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="E22" s="0" t="s">
+      <c r="F22" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591444ca-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="G22" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917acf0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>97</v>
       </c>
       <c r="I22" s="0" t="s">
         <v>53</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="B23" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591720a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H23" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="C23" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="E23" s="0" t="s">
+      <c r="I23" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="F23" s="0" t="s">
+      <c r="J23" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="G23" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590de58a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H23" s="0" t="s">
+      <c r="K23" s="0" t="s">
         <v>103</v>
-      </c>
-      <c r="I23" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="J23" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="K23" s="0" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="B24" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="C24" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="E24" s="0" t="s">
+      <c r="F24" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="F24" s="0" t="s">
-        <v>96</v>
-      </c>
       <c r="G24" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59147b48-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59177dc0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="H24" s="0" t="s">
@@ -1287,441 +1280,336 @@
         <v>108</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="G25" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591444ca-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591306a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I25" s="0" t="s">
         <v>53</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="F26" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591720a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H26" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="I26" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="J26" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="K26" s="0" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="B27" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/41455e80-4f40-11e6-a814-ac72891c3257.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="J27" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="K27" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E29" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="C27" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="E27" s="0" t="s">
+      <c r="F29" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="F27" s="0" t="s">
+      <c r="G29" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/9c35e2ac-a0de-11e6-bc63-ac72891c3257.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H29" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="G27" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59177dc0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H27" s="0" t="s">
+      <c r="I29" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="J29" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="I27" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="J27" s="0" t="s">
+      <c r="K29" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="K27" s="0" t="s">
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="B28" s="0" t="s">
+      <c r="B31" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="C28" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="E28" s="0" t="s">
+      <c r="C31" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="F28" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="G28" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591306a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H28" s="0" t="s">
+      <c r="E31" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="I28" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="J28" s="0" t="s">
+      <c r="F31" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="K28" s="0" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="I31" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="J31" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="B30" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="F30" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="G30" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/41455e80-4f40-11e6-a814-ac72891c3257.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H30" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="I30" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="J30" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="K30" s="0" t="s">
-        <v>66</v>
+      <c r="K31" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="I32" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="J32" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="K32" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B33" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="C33" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="E33" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="C32" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D32" s="0" t="s">
+      <c r="F33" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/53826ae4-bf01-11e6-a554-ac72891c3257.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H33" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="E32" s="0" t="s">
+      <c r="I33" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="J33" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="F32" s="0" t="s">
+      <c r="K33" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="G32" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/9c35e2ac-a0de-11e6-bc63-ac72891c3257.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H32" s="0" t="s">
+      <c r="B38" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="I32" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="J32" s="0" t="s">
+      <c r="C38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E38" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="K32" s="0" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="F34" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="G34" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H34" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="I34" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="J34" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="K34" s="0" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="G35" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H35" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I35" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="J35" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="K35" s="0" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="F36" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="G36" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/53826ae4-bf01-11e6-a554-ac72891c3257.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H36" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="I36" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="J36" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="K36" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="B41" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="F41" s="0" t="s">
+      <c r="F38" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="G41" s="0" t="str">
+      <c r="G38" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/865d0e00-53e6-11e6-b524-5404a60d96b5.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H41" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="J41" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="K41" s="0" t="s">
+      <c r="H38" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J38" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="K38" s="0" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="B42" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="E42" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="F42" s="0" t="s">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="F39" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="G42" s="0" t="str">
+      <c r="G39" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H42" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="I42" s="2" t="s">
+      <c r="H39" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I39" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="J42" s="0" t="s">
+      <c r="J39" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="K39" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="K42" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="B43" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="F43" s="0" t="s">
+      <c r="E40" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="F40" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="G43" s="0" t="str">
+      <c r="G40" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H43" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="I43" s="2" t="s">
+      <c r="H40" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I40" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="J43" s="0" t="s">
+      <c r="J40" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="K43" s="0" t="s">
+      <c r="K40" s="0" t="s">
         <v>66</v>
       </c>
     </row>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>

<commit_message>
The variables nudgincsm & nudgincswe needed to be added to the identified missing list after the merge of the grib_table_126 branch into the master to get the genecec output correct #450 #368.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables-enable-pextra.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables-enable-pextra.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="157">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -461,6 +461,94 @@
   </si>
   <si>
     <t xml:space="preserve">For Greenland this is the same as sftgif. We do not have an Antarctic ice sheet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nudgincsm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nudging Increment of Water in Soil Moisture</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">To be implemented: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE181E"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> grib 126.151</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">:  ifs code name = 151.126  part of MFPPHY.  Have to be  made available via PEXTRA, upto now with some  non-defined or adhoc grib code. Nudincsm is, consistent with sm, saved for each of the four soil layers</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Emanuel Dutra, Wilhelm May, Thomas Reerink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A nudging increment refers to an amount added to parts of a model system. The phrase 'nudging_increment_in_X' refers to an increment in quantity X over a time period which should be defined in the bounds of the time coordinate. 'Content' indicates a quantity per unit area. 'Water' means water in all phases. The mass content of water in soil refers to the vertical integral from the surface down to the bottom of the soil model. The 'soil content' of a quantity refers to the vertical integral from the surface down to the bottom of the soil model. For the content between specified levels in the soil, standard names including 'content_of_soil_layer' are used.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nudgincswe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nudging Increment of Water in Snow</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">To be implemented:  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE181E"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">grib 126.152</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">:  ifs code name = 152.126  part of MFPPHY.  Have to be  made available via PEXTRA, upto now with some  non-defined or adhoc grib code.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">A nudging increment refers to an amount added to parts of a model system. The phrase 'nudging_increment_in_X' refers to an increment in quantity X over a time period which should be defined in the bounds of the time coordinate. The surface called 'surface' means the lower boundary of the atmosphere. 'Amount' means mass per unit area. 'Snow and ice on land' means ice in glaciers, ice caps, ice sheets &amp; shelves, river and lake ice, any other ice on a land surface, such as frozen flood water, and snow lying on such ice or on the land surface.</t>
   </si>
 </sst>
 </file>
@@ -470,7 +558,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -497,6 +585,13 @@
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCE181E"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -566,6 +661,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCE181E"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -576,8 +731,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B47" activeCellId="0" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1607,6 +1762,78 @@
         <v>66</v>
       </c>
     </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G43" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/01c8c41a-a0d8-11e6-bc63-ac72891c3257.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H43" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="I43" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="J43" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="K43" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G44" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0abbdddc-a0d8-11e6-bc63-ac72891c3257.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H44" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="I44" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="J44" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="K44" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Taking Efx slthick off from the identified missing list, so it can be cmorised #439.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables-enable-pextra.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables-enable-pextra.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="152">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -169,103 +169,88 @@
     <t xml:space="preserve">Volume fraction of silt in soil</t>
   </si>
   <si>
-    <t xml:space="preserve">slthick</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thickness of Soil Layers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Available in IFS: independent of lon, lat. Top soil layer: 0-7 cm, Soil layer 2: 7-28 cm, Soil layer 3: 28-100 cm, Soil layer 4: 100-289 cm, added as issue #126</t>
+    <t xml:space="preserve">wilt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wilting Point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wilting point is defined in HTESSEL as a fraction (different for each soil texture in HTESSEL; variable slt grib code 43 - Table 128) of field capacity. (Alessandri A.: an Effective Wilting Point can be defined ... same as below discussion for the field capacity)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage water content of soil by volume at the wilting point. The wilting point of soil is the water content below which plants cannot extract sufficient water to balance their loss through transpiration. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IfxGre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">areacellg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grid-Cell Area for Ice Sheet Variables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To be implemented:  grib 126.34  part of MFPPHY   Available in PISM. This is the ice sheet mask (in fraction) defined in the ice sheet model grid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Area of the target grid (not the interpolated area of the source grid).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISMIP6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ImonGre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mrroLi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xgre ygre time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Land Ice Runoff Flux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kg m-2 s-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IFS Surface runoff grib 128.8 but for EC_Earth-GrIs additional melt etc is included</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shuting, Thomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Runoff flux over land ice is the difference between any available liquid water in the snowpack less any refreezing. Computed as the sum of rainfall and melt of snow or ice less any refreezing or water retained in the snowpack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IfxAnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intuadse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertically Integrated Eastward Dry Statice Energy Transport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MJ m-1 s-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in the standard IFS output. However, per layer the specific heat capacity of dry air (1005.7 J kg-1 K-1) can be multiplied by the Temperature (grib 128.130) times the V component of wind (grib 128.132) + the geopotential height  (grib 128.129) and this needs to be vertically integrated times the air density per layer.</t>
   </si>
   <si>
     <t xml:space="preserve">Gijs &amp; Thomas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">'Thickness' means the vertical extent of a layer. 'Cell' refers to a model grid cell.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wilt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wilting Point</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wilting point is defined in HTESSEL as a fraction (different for each soil texture in HTESSEL; variable slt grib code 43 - Table 128) of field capacity. (Alessandri A.: an Effective Wilting Point can be defined ... same as below discussion for the field capacity)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage water content of soil by volume at the wilting point. The wilting point of soil is the water content below which plants cannot extract sufficient water to balance their loss through transpiration. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IfxGre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">areacellg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">longitude latitude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grid-Cell Area for Ice Sheet Variables</t>
-  </si>
-  <si>
-    <t xml:space="preserve">m2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To be implemented:  grib 126.34  part of MFPPHY   Available in PISM. This is the ice sheet mask (in fraction) defined in the ice sheet model grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Area of the target grid (not the interpolated area of the source grid).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ISMIP6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ImonGre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrroLi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xgre ygre time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Land Ice Runoff Flux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kg m-2 s-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IFS Surface runoff grib 128.8 but for EC_Earth-GrIs additional melt etc is included</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shuting, Thomas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Runoff flux over land ice is the difference between any available liquid water in the snowpack less any refreezing. Computed as the sum of rainfall and melt of snow or ice less any refreezing or water retained in the snowpack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IfxAnt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Emon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">intuadse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">longitude latitude time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vertically Integrated Eastward Dry Statice Energy Transport</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MJ m-1 s-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not available in the standard IFS output. However, per layer the specific heat capacity of dry air (1005.7 J kg-1 K-1) can be multiplied by the Temperature (grib 128.130) times the V component of wind (grib 128.132) + the geopotential height  (grib 128.129) and this needs to be vertically integrated times the air density per layer.</t>
   </si>
   <si>
     <t xml:space="preserve">Vertically integrated eastward dry static energy transport (cp.T +zg).v (Mass_weighted_vertical integral of the product of eastward wind by dry static_energy per mass unit)</t>
@@ -731,8 +716,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B47" activeCellId="0" sqref="B47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1056,211 +1041,211 @@
         <v>50</v>
       </c>
       <c r="F10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7124926c-c7b6-11e6-bb2a-ac72891c3257.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="G10" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7124901e-c7b6-11e6-bb2a-ac72891c3257.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="0" t="s">
+      <c r="I10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="I10" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="J10" s="0" t="s">
-        <v>54</v>
       </c>
       <c r="K10" s="0" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="0" t="s">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="0" t="s">
+      <c r="E12" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7124926c-c7b6-11e6-bb2a-ac72891c3257.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H11" s="0" t="s">
+      <c r="F12" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="I11" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="J11" s="0" t="s">
+      <c r="G12" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e9b495e2-5989-11e6-a4be-ac72891c3257.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="K11" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="I12" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="K12" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="0" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="B14" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="C14" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="E14" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/41455e80-4f40-11e6-a814-ac72891c3257.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" s="0" t="n">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e9b495e2-5989-11e6-a4be-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
-      <c r="H13" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="I13" s="0" t="s">
+      <c r="H16" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="I16" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="J13" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="K13" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" s="0" t="s">
+      <c r="J16" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="K16" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="B18" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="G15" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/41455e80-4f40-11e6-a814-ac72891c3257.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="0" t="s">
+      <c r="C18" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="I15" s="0" t="s">
+      <c r="E18" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="J15" s="0" t="s">
+      <c r="F18" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="K15" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="G18" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917acf0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="G17" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e9b495e2-5989-11e6-a4be-ac72891c3257.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="K17" s="0" t="s">
-        <v>66</v>
+      <c r="I18" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="K18" s="0" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590de58a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="I19" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="B19" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="0" t="s">
+      <c r="J19" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="K19" s="0" t="s">
         <v>78</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="G19" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917acf0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="I19" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="J19" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="K19" s="0" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>84</v>
@@ -1269,314 +1254,314 @@
         <v>13</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E20" s="0" t="s">
         <v>85</v>
       </c>
       <c r="F20" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59147b48-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="G20" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590de58a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H20" s="0" t="s">
+      <c r="I20" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="J20" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="I20" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="J20" s="0" t="s">
-        <v>88</v>
-      </c>
       <c r="K20" s="0" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591444ca-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="I21" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="B21" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="0" t="s">
+      <c r="J21" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="K21" s="0" t="s">
         <v>78</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="G21" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59147b48-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H21" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="J21" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="K21" s="0" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B22" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="0" t="s">
         <v>93</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>78</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>94</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>86</v>
+        <v>13</v>
       </c>
       <c r="G22" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591444ca-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591720a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="H22" s="0" t="s">
         <v>95</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59177dc0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="I23" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="B23" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591720a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="I23" s="0" t="s">
-        <v>101</v>
-      </c>
       <c r="J23" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="G24" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59177dc0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591306a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="H24" s="0" t="s">
         <v>107</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="J24" s="0" t="s">
         <v>108</v>
       </c>
       <c r="K24" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="B26" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/41455e80-4f40-11e6-a814-ac72891c3257.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="I26" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="J26" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="K26" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/9c35e2ac-a0de-11e6-bc63-ac72891c3257.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="I28" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="B25" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="G25" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591306a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H25" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="I25" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="J25" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="K25" s="0" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="F27" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="G27" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/41455e80-4f40-11e6-a814-ac72891c3257.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H27" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="I27" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="J27" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="K27" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="B29" s="0" t="s">
+      <c r="J28" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="C29" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="0" t="s">
+      <c r="K28" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="E29" s="0" t="s">
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="F29" s="0" t="s">
+      <c r="B30" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="G29" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/9c35e2ac-a0de-11e6-bc63-ac72891c3257.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H29" s="0" t="s">
+      <c r="C30" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="I29" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="J29" s="0" t="s">
+      <c r="E30" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="K29" s="0" t="s">
+      <c r="F30" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="0" t="s">
         <v>123</v>
+      </c>
+      <c r="I30" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="J30" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="K30" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B31" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="C31" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>126</v>
-      </c>
       <c r="E31" s="0" t="s">
-        <v>127</v>
+        <v>40</v>
       </c>
       <c r="F31" s="0" t="s">
         <v>22</v>
       </c>
       <c r="G31" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>128</v>
+        <v>41</v>
       </c>
       <c r="I31" s="0" t="s">
         <v>42</v>
       </c>
       <c r="J31" s="0" t="s">
-        <v>129</v>
+        <v>43</v>
       </c>
       <c r="K31" s="0" t="s">
         <v>44</v>
@@ -1584,187 +1569,187 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>38</v>
+        <v>126</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>130</v>
+        <v>72</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>40</v>
+        <v>127</v>
       </c>
       <c r="F32" s="0" t="s">
         <v>22</v>
       </c>
       <c r="G32" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/53826ae4-bf01-11e6-a554-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>41</v>
+        <v>128</v>
       </c>
       <c r="I32" s="0" t="s">
         <v>42</v>
       </c>
       <c r="J32" s="0" t="s">
-        <v>43</v>
+        <v>129</v>
       </c>
       <c r="K32" s="0" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="B33" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B37" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="C33" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="E33" s="0" t="s">
+      <c r="C37" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E37" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="F33" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="G33" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/53826ae4-bf01-11e6-a554-ac72891c3257.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H33" s="0" t="s">
+      <c r="F37" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="G37" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/865d0e00-53e6-11e6-b524-5404a60d96b5.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H37" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="I33" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="J33" s="0" t="s">
+      <c r="I37" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="K33" s="0" t="s">
-        <v>66</v>
+      <c r="J37" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="K37" s="0" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B38" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="0" t="s">
         <v>136</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D38" s="0" t="s">
-        <v>69</v>
       </c>
       <c r="E38" s="0" t="s">
         <v>137</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
       <c r="G38" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/865d0e00-53e6-11e6-b524-5404a60d96b5.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
         <v>web</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>138</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>139</v>
+        <v>67</v>
       </c>
       <c r="J38" s="0" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="K38" s="0" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>125</v>
+        <v>38</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F39" s="0" t="s">
         <v>22</v>
       </c>
       <c r="G39" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="J39" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="K39" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="B40" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D40" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="E40" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="F40" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="G40" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="H39" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J39" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="K39" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G42" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/01c8c41a-a0d8-11e6-bc63-ac72891c3257.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H42" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="I42" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="I40" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="J40" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="K40" s="0" t="s">
-        <v>66</v>
+      <c r="J42" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="K42" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>148</v>
@@ -1773,7 +1758,7 @@
         <v>13</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E43" s="0" t="s">
         <v>149</v>
@@ -1782,58 +1767,23 @@
         <v>32</v>
       </c>
       <c r="G43" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/01c8c41a-a0d8-11e6-bc63-ac72891c3257.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0abbdddc-a0d8-11e6-bc63-ac72891c3257.html","web")</f>
         <v>web</v>
       </c>
       <c r="H43" s="0" t="s">
         <v>150</v>
       </c>
       <c r="I43" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="J43" s="0" t="s">
         <v>151</v>
-      </c>
-      <c r="J43" s="0" t="s">
-        <v>152</v>
       </c>
       <c r="K43" s="0" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D44" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="F44" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="G44" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0abbdddc-a0d8-11e6-bc63-ac72891c3257.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H44" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="I44" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="J44" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="K44" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
The Amon o3 combination will be added to the pextra identified missing list in order to prevent IFS crashes, and to pave the way for release 1.0.0 #458 #440.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables-enable-pextra.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables-enable-pextra.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="161">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -534,6 +534,33 @@
   </si>
   <si>
     <t xml:space="preserve">A nudging increment refers to an amount added to parts of a model system. The phrase 'nudging_increment_in_X' refers to an increment in quantity X over a time period which should be defined in the bounds of the time coordinate. The surface called 'surface' means the lower boundary of the atmosphere. 'Amount' means mass per unit area. 'Snow and ice on land' means ice in glaciers, ice caps, ice sheets &amp; shelves, river and lake ice, any other ice on a land surface, such as frozen flood water, and snow lying on such ice or on the land surface.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude plev19 time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mole Fraction of O3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mol mol-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tm5 code name = o3|ifs code name = 203.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">automatic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mole fraction is used in the construction mole_fraction_of_X_in_Y, where X is a material constituent of Y.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AerChemMIP,C4MIP,CFMIP,CMIP,DAMIP,FAFMIP,GMMIP,GeoMIP,HighResMIP,LS3MIP,LUMIP,RFMIP,VolMIP</t>
   </si>
 </sst>
 </file>
@@ -716,8 +743,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A46" activeCellId="0" sqref="46:46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1783,6 +1810,42 @@
         <v>19</v>
       </c>
     </row>
+    <row r="46" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G46" s="2" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/1d4594c97188efd47935238a429e02e4.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Update also the pextra variant of the identified missing list #526.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables-enable-pextra.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables-enable-pextra.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="140">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">1</t>
   </si>
   <si>
-    <t xml:space="preserve">longitude latitude typegis</t>
+    <t xml:space="preserve">longitude latitude</t>
   </si>
   <si>
     <t xml:space="preserve">Grounded Ice Sheet Area Percentage</t>
@@ -79,268 +79,268 @@
     <t xml:space="preserve">Shuting</t>
   </si>
   <si>
+    <t xml:space="preserve">Percentage of grid cell covered by grounded ice sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMIP,ISMIP6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IfxGre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">areacellg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grid-Cell Area for Ice Sheet Variables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To be implemented:  grib 126.34  part of MFPPHY   Available in PISM. This is the ice sheet mask (in fraction) defined in the ice sheet model grid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Area of the target grid (not the interpolated area of the source grid).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISMIP6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ImonGre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mrroLi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xgre ygre time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Land Ice Runoff Flux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kg m-2 s-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IFS Surface runoff grib 128.8 but for EC_Earth-GrIs additional melt etc is included</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shuting, Thomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Runoff flux over land ice is the difference between any available liquid water in the snowpack less any refreezing. Computed as the sum of rainfall and melt of snow or ice less any refreezing or water retained in the snowpack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intuadse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertically Integrated Eastward Dry Statice Energy Transport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MJ m-1 s-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in the standard IFS output. However, per layer the specific heat capacity of dry air (1005.7 J kg-1 K-1) can be multiplied by the Temperature (grib 128.130) times the V component of wind (grib 128.132) + the geopotential height  (grib 128.129) and this needs to be vertically integrated times the air density per layer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gijs &amp; Thomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertically integrated eastward dry static energy transport (cp.T +zg).v (Mass_weighted_vertical integral of the product of eastward wind by dry static_energy per mass unit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intuaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertically Integrated Eastward Moisture Transport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kg m-1 s-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in the standard IFS output. However, per layer the Specific humidity (grib 128.133 + unit conversion) can be multiplied by the U component of wind (grib 128.131) and this needs to be vertically integrated.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertically integrated Eastward moisture transport (Mass weighted vertical integral of the product of eastward wind by total water mass per unit mass)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intvadse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertically Integrated Northward Dry Static Energy Transport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in the standard IFS output. However, per layer the specific heat capacity of dry air (1005.7 J kg-1 K-1) can be multiplied by the Temperature (grib 128.130) times the U component of wind (grib 128.131) + the geopotential height  (grib 128.129) and this needs to be vertically integrated times the air density per layer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertically integrated northward dry static energy transport (cp.T +zg).v (Mass_weighted_vertical integral of the product of northward wind by dry static_energy per mass unit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intvaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertically Integrated Northward Moisture Transport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in the standard IFS output. However, per layer the Specific humidity (grib 128.133 + unit conversion) can be multiplied by the V component of wind (grib 128.132) and this needs to be vertically integrated.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertically integrated Northward moisture transport (Mass_weighted_vertical integral of the product of northward wind by total water mass per unit mass)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">od550aerso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude time lambda550nm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stratospheric Optical Depth at 550nm (All Aerosols) 2D-Field (Stratosphere Only)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Determined by CMIP6 stratospheric aerosol forcing data set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twan &amp; Thomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From tropopause to stratopause as defined by the model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GeoMIP,PMIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uqint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eastward Humidity Transport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m2 s-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in IFS, via postprocessing the vertical integral can be taken of the following grib 128.131 * 128.133</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column integrated eastward wind times specific humidity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HighResMIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vqint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northward Humidity Transport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available in IFS, via postprocessing the vertical integral can be taken of the following grib 128.132 * 128.133</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column integrated northward wind times specific humidity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E3hrPt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude time1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solar Zenith Angle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">degree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the IFS code we found: A CALL TO SUBROUTINE *SOLANG* GIVES FIELDS OF SOLAR ZENITH. Best would be to copy the IFS routine/formula to ece2cmor3 and produce this field off-line.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The angle between the line of sight to the sun and the local vertical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RFMIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LImon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sftgif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Land Ice Area Percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To be implemented:  grib 126.32  part of MFPPHY   This is the land ice mask and will be an extra variable in IFS (thomas: via PEXTRA?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage of grid cell covered by land ice (ice sheet, ice shelf, ice cap, glacier)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sncIs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ice Sheet Snow Cover Percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To be implemented:  grib 126.31  part of MFPPHY   Not available in IFS. Although it could be calculated from tile fractions and written out as extra output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage of each grid cell that is occupied by snow that rests on land portion of cell.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IyrGre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modelCellAreai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cell area of the ice sheet model.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">web</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The PISM model probably uses a constant and uniform grid size within EC-Earth, this grid size can be reported or a filed from the grid sizes can be provided in a post processing phase.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horizontal area of ice-sheet grid cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xgre ygre time typeli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fraction of Grid Cell Covered with Glacier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is the land ice mask and will be an extra variable in IFS (thomas: via PEXTRA?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fraction of grid cell covered by land ice (ice sheet, ice shelf, ice cap, glacier)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xgre ygre time typegis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grounded Ice Sheet  Area Fraction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For Greenland this is the same as sftgif. We do not have an Antarctic ice sheet.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fraction of grid cell covered by grounded ice sheet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CMIP,ISMIP6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IfxGre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">areacellg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">longitude latitude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grid-Cell Area for Ice Sheet Variables</t>
-  </si>
-  <si>
-    <t xml:space="preserve">m2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To be implemented:  grib 126.34  part of MFPPHY   Available in PISM. This is the ice sheet mask (in fraction) defined in the ice sheet model grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Area of the target grid (not the interpolated area of the source grid).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ISMIP6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ImonGre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrroLi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xgre ygre time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Land Ice Runoff Flux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kg m-2 s-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IFS Surface runoff grib 128.8 but for EC_Earth-GrIs additional melt etc is included</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shuting, Thomas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Runoff flux over land ice is the difference between any available liquid water in the snowpack less any refreezing. Computed as the sum of rainfall and melt of snow or ice less any refreezing or water retained in the snowpack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Emon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">intuadse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">longitude latitude time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vertically Integrated Eastward Dry Statice Energy Transport</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MJ m-1 s-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not available in the standard IFS output. However, per layer the specific heat capacity of dry air (1005.7 J kg-1 K-1) can be multiplied by the Temperature (grib 128.130) times the V component of wind (grib 128.132) + the geopotential height  (grib 128.129) and this needs to be vertically integrated times the air density per layer.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gijs &amp; Thomas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vertically integrated eastward dry static energy transport (cp.T +zg).v (Mass_weighted_vertical integral of the product of eastward wind by dry static_energy per mass unit)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PMIP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">intuaw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vertically Integrated Eastward Moisture Transport</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kg m-1 s-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not available in the standard IFS output. However, per layer the Specific humidity (grib 128.133 + unit conversion) can be multiplied by the U component of wind (grib 128.131) and this needs to be vertically integrated.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vertically integrated Eastward moisture transport (Mass weighted vertical integral of the product of eastward wind by total water mass per unit mass)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">intvadse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vertically Integrated Northward Dry Static Energy Transport</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not available in the standard IFS output. However, per layer the specific heat capacity of dry air (1005.7 J kg-1 K-1) can be multiplied by the Temperature (grib 128.130) times the U component of wind (grib 128.131) + the geopotential height  (grib 128.129) and this needs to be vertically integrated times the air density per layer.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vertically integrated northward dry static energy transport (cp.T +zg).v (Mass_weighted_vertical integral of the product of northward wind by dry static_energy per mass unit)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">intvaw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vertically Integrated Northward Moisture Transport</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not available in the standard IFS output. However, per layer the Specific humidity (grib 128.133 + unit conversion) can be multiplied by the V component of wind (grib 128.132) and this needs to be vertically integrated.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vertically integrated Northward moisture transport (Mass_weighted_vertical integral of the product of northward wind by total water mass per unit mass)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">od550aerso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">longitude latitude time lambda550nm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stratospheric Optical Depth at 550nm (All Aerosols) 2D-Field (Stratosphere Only)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Determined by CMIP6 stratospheric aerosol forcing data set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Twan &amp; Thomas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">From tropopause to stratopause as defined by the model</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GeoMIP,PMIP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uqint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eastward Humidity Transport</t>
-  </si>
-  <si>
-    <t xml:space="preserve">m2 s-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Available in IFS, via postprocessing the vertical integral can be taken of the following grib 128.131 * 128.133</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column integrated eastward wind times specific humidity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HighResMIP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vqint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Northward Humidity Transport</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Available in IFS, via postprocessing the vertical integral can be taken of the following grib 128.132 * 128.133</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column integrated northward wind times specific humidity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E3hrPt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sza</t>
-  </si>
-  <si>
-    <t xml:space="preserve">longitude latitude time1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solar Zenith Angle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">degree</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In the IFS code we found: A CALL TO SUBROUTINE *SOLANG* GIVES FIELDS OF SOLAR ZENITH. Best would be to copy the IFS routine/formula to ece2cmor3 and produce this field off-line.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The angle between the line of sight to the sun and the local vertical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RFMIP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LImon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sftgif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">longitude latitude time typeli</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Land Ice Area Percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To be implemented:  grib 126.32  part of MFPPHY   This is the land ice mask and will be an extra variable in IFS (thomas: via PEXTRA?)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fraction of grid cell covered by land ice (ice sheet, ice shelf, ice cap, glacier)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">longitude latitude time typegis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sncIs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ice Sheet Snow Cover Percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To be implemented:  grib 126.31  part of MFPPHY   Not available in IFS. Although it could be calculated from tile fractions and written out as extra output</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage of each grid cell that is occupied by snow that rests on land portion of cell.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IyrGre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">modelCellAreai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The cell area of the ice sheet model.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The PISM model probably uses a constant and uniform grid size within EC-Earth, this grid size can be reported or a filed from the grid sizes can be provided in a post processing phase.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thomas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Horizontal area of ice-sheet grid cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xgre ygre time typeli</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fraction of Grid Cell Covered with Glacier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is the land ice mask and will be an extra variable in IFS (thomas: via PEXTRA?)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xgre ygre time typegis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grounded Ice Sheet  Area Fraction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For Greenland this is the same as sftgif. We do not have an Antarctic ice sheet.</t>
   </si>
   <si>
     <t xml:space="preserve">Eday</t>
@@ -443,9 +443,6 @@
     <t xml:space="preserve">Total Soil Wetness</t>
   </si>
   <si>
-    <t xml:space="preserve">web</t>
-  </si>
-  <si>
     <t xml:space="preserve">mrsow=swvl1*0.07+swvl2*0.21+swvl3*0.72+swvl4*1.89 note: NOT divided by maximum allowable soil moisture above wilting point</t>
   </si>
   <si>
@@ -495,6 +492,12 @@
   </si>
   <si>
     <t xml:space="preserve">AerChemMIP,C4MIP,CFMIP,CMIP,DAMIP,FAFMIP,GMMIP,GeoMIP,HighResMIP,LS3MIP,LUMIP,RFMIP,VolMIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude time typeli</t>
   </si>
 </sst>
 </file>
@@ -585,16 +588,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -677,8 +676,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B42" activeCellId="0" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -751,9 +750,9 @@
       <c r="F3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="0" t="str">
+      <c r="G3" s="0" t="n">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>web</v>
+        <v>0</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>17</v>
@@ -779,386 +778,386 @@
         <v>13</v>
       </c>
       <c r="D5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="F5" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="G5" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e9b495e2-5989-11e6-a4be-ac72891c3257.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="G5" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e9b495e2-5989-11e6-a4be-ac72891c3257.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>26</v>
       </c>
       <c r="I5" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="C7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="0" t="s">
+      <c r="E7" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="F7" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="G7" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/41455e80-4f40-11e6-a814-ac72891c3257.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/41455e80-4f40-11e6-a814-ac72891c3257.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H7" s="0" t="s">
+      <c r="I7" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="J7" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="K7" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="C9" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="0" t="s">
+      <c r="E9" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="F9" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="G9" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917acf0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917acf0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H9" s="0" t="s">
+      <c r="I9" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="I9" s="0" t="s">
+      <c r="J9" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="J9" s="0" t="s">
+      <c r="K9" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="K9" s="0" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="0" t="s">
+      <c r="F10" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="G10" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590de58a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590de58a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H10" s="0" t="s">
+      <c r="I10" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="I10" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="J10" s="0" t="s">
-        <v>50</v>
-      </c>
       <c r="K10" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="0" t="s">
+      <c r="F11" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59147b48-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59147b48-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H11" s="0" t="s">
+      <c r="I11" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="I11" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>54</v>
-      </c>
       <c r="K11" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="0" t="s">
+      <c r="F12" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591444ca-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591444ca-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H12" s="0" t="s">
+      <c r="I12" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="I12" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="J12" s="0" t="s">
-        <v>58</v>
-      </c>
       <c r="K12" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="0" t="s">
+      <c r="E13" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="F13" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591720a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="F13" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591720a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H13" s="0" t="s">
+      <c r="I13" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="I13" s="0" t="s">
+      <c r="J13" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="J13" s="0" t="s">
+      <c r="K13" s="0" t="s">
         <v>64</v>
-      </c>
-      <c r="K13" s="0" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="0" t="s">
+      <c r="F14" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="G14" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59177dc0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="G14" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59177dc0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H14" s="0" t="s">
+      <c r="I14" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="I14" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="J14" s="0" t="s">
+      <c r="K14" s="0" t="s">
         <v>70</v>
-      </c>
-      <c r="K14" s="0" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="0" t="s">
+      <c r="F15" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591306a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="G15" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591306a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H15" s="0" t="s">
+      <c r="I15" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="J15" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="I15" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="J15" s="0" t="s">
-        <v>75</v>
-      </c>
       <c r="K15" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="C17" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="C17" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="0" t="s">
+      <c r="E17" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="F17" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="F17" s="0" t="s">
+      <c r="G17" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/9c35e2ac-a0de-11e6-bc63-ac72891c3257.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="G17" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/9c35e2ac-a0de-11e6-bc63-ac72891c3257.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H17" s="0" t="s">
+      <c r="I17" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="J17" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="I17" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="J17" s="0" t="s">
+      <c r="K17" s="0" t="s">
         <v>82</v>
-      </c>
-      <c r="K17" s="0" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="C19" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="0" t="s">
         <v>85</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>87</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G19" s="0" t="str">
+      <c r="G19" s="0" t="n">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
-        <v>web</v>
+        <v>0</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I19" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K19" s="0" t="s">
         <v>20</v>
@@ -1166,7 +1165,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>12</v>
@@ -1175,7 +1174,7 @@
         <v>13</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>90</v>
+        <v>38</v>
       </c>
       <c r="E20" s="0" t="s">
         <v>15</v>
@@ -1183,9 +1182,9 @@
       <c r="F20" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="0" t="str">
+      <c r="G20" s="0" t="n">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>web</v>
+        <v>0</v>
       </c>
       <c r="H20" s="0" t="s">
         <v>17</v>
@@ -1202,115 +1201,113 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G21" s="0" t="str">
+      <c r="G21" s="0" t="n">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/53826ae4-bf01-11e6-a554-ac72891c3257.html","web")</f>
-        <v>web</v>
+        <v>0</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="I21" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="H26" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="C26" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E26" s="0" t="s">
+      <c r="I26" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="F26" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="G26" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/865d0e00-53e6-11e6-b524-5404a60d96b5.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H26" s="2" t="s">
+      <c r="J26" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="I26" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="J26" s="0" t="s">
-        <v>100</v>
-      </c>
       <c r="K26" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G27" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>35</v>
+      <c r="G27" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>12</v>
@@ -1319,29 +1316,28 @@
         <v>13</v>
       </c>
       <c r="D28" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E28" s="0" t="s">
         <v>104</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>105</v>
       </c>
       <c r="F28" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G28" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H28" s="2" t="s">
+      <c r="G28" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J28" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="I28" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J28" s="0" t="s">
-        <v>19</v>
-      </c>
       <c r="K28" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1355,7 +1351,7 @@
         <v>13</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E31" s="0" t="s">
         <v>109</v>
@@ -1363,9 +1359,8 @@
       <c r="F31" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="G31" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/01c8c41a-a0d8-11e6-bc63-ac72891c3257.html","web")</f>
-        <v>web</v>
+      <c r="G31" s="0" t="s">
+        <v>95</v>
       </c>
       <c r="H31" s="0" t="s">
         <v>111</v>
@@ -1391,7 +1386,7 @@
         <v>13</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E32" s="0" t="s">
         <v>116</v>
@@ -1399,9 +1394,8 @@
       <c r="F32" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="G32" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0abbdddc-a0d8-11e6-bc63-ac72891c3257.html","web")</f>
-        <v>web</v>
+      <c r="G32" s="0" t="s">
+        <v>95</v>
       </c>
       <c r="H32" s="0" t="s">
         <v>117</v>
@@ -1427,7 +1421,7 @@
         <v>13</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E35" s="0" t="s">
         <v>120</v>
@@ -1436,16 +1430,16 @@
         <v>13</v>
       </c>
       <c r="G35" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="H35" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="H35" s="0" t="s">
+      <c r="I35" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="I35" s="0" t="s">
+      <c r="J35" s="0" t="s">
         <v>123</v>
-      </c>
-      <c r="J35" s="0" t="s">
-        <v>124</v>
       </c>
       <c r="K35" s="0" t="s">
         <v>114</v>
@@ -1456,72 +1450,144 @@
         <v>107</v>
       </c>
       <c r="B36" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E36" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="C36" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="E36" s="0" t="s">
+      <c r="F36" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="F36" s="0" t="s">
+      <c r="G36" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="H36" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="G36" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="H36" s="0" t="s">
+      <c r="I36" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="J36" s="0" t="s">
         <v>128</v>
-      </c>
-      <c r="I36" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="J36" s="0" t="s">
-        <v>129</v>
       </c>
       <c r="K36" s="0" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="39" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="2" t="s">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B39" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="C39" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D39" s="2" t="s">
+      <c r="E39" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="F39" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="G39" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="H39" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="G39" s="2" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/1d4594c97188efd47935238a429e02e4.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H39" s="2" t="s">
+      <c r="I39" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="I39" s="2" t="s">
+      <c r="J39" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="J39" s="2" t="s">
+      <c r="K39" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="K39" s="2" t="s">
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
         <v>138</v>
       </c>
-    </row>
+      <c r="B42" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G42" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="H42" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="I42" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J42" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="K42" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Update the identified missing list for the pextra including case #554, #521, #394.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables-enable-pextra.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables-enable-pextra.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="130">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -435,36 +435,6 @@
   </si>
   <si>
     <t xml:space="preserve">A nudging increment refers to an amount added to parts of a model system. The phrase 'nudging_increment_in_X' refers to an increment in quantity X over a time period which should be defined in the bounds of the time coordinate. The surface called 'surface' means the lower boundary of the atmosphere. 'Amount' means mass per unit area. 'Snow and ice on land' means ice in glaciers, ice caps, ice sheets &amp; shelves, river and lake ice, any other ice on a land surface, such as frozen flood water, and snow lying on such ice or on the land surface.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrsow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Soil Wetness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrsow=swvl1*0.07+swvl2*0.21+swvl3*0.72+swvl4*1.89 note: NOT divided by maximum allowable soil moisture above wilting point</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Andrea Alessandri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vertically integrated soil moisture divided by maximum allowable soil moisture above wilting point.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tsland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Land Surface Temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Available by IFS: grib code 235 but it needs masking out the ocean points: thus add in ifspar.json the entry "masked": "land"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperature of the lower boundary of the atmosphere</t>
   </si>
   <si>
     <t xml:space="preserve">Amon</t>
@@ -676,11 +646,11 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B42" activeCellId="0" sqref="B42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
@@ -696,7 +666,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -731,7 +701,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>11</v>
       </c>
@@ -767,7 +737,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>21</v>
       </c>
@@ -803,7 +773,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>28</v>
       </c>
@@ -839,7 +809,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>36</v>
       </c>
@@ -875,7 +845,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>36</v>
       </c>
@@ -911,7 +881,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>36</v>
       </c>
@@ -947,7 +917,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>36</v>
       </c>
@@ -983,7 +953,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>36</v>
       </c>
@@ -1019,7 +989,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>36</v>
       </c>
@@ -1055,7 +1025,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>36</v>
       </c>
@@ -1091,7 +1061,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>75</v>
       </c>
@@ -1127,7 +1097,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>83</v>
       </c>
@@ -1163,7 +1133,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>83</v>
       </c>
@@ -1199,7 +1169,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>83</v>
       </c>
@@ -1235,178 +1205,152 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B29" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="C26" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="0" t="s">
+      <c r="C29" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E26" s="0" t="s">
+      <c r="E29" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="F26" s="0" t="s">
+      <c r="F29" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="G26" s="0" t="s">
+      <c r="G29" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="H26" s="0" t="s">
+      <c r="H29" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="I26" s="0" t="s">
+      <c r="I29" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="J26" s="0" t="s">
+      <c r="J29" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="K26" s="0" t="s">
+      <c r="K29" s="0" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B30" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="0" t="s">
+      <c r="C30" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="E27" s="0" t="s">
+      <c r="E30" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="F27" s="0" t="s">
+      <c r="F30" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G27" s="0" t="s">
+      <c r="G30" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="H27" s="0" t="s">
+      <c r="H30" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="I27" s="0" t="s">
+      <c r="I30" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="J27" s="0" t="s">
+      <c r="J30" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="K27" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="F28" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G28" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="H28" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="I28" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="J28" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="K28" s="0" t="s">
+      <c r="K30" s="0" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>108</v>
+        <v>12</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>38</v>
+        <v>103</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>110</v>
+        <v>16</v>
       </c>
       <c r="G31" s="0" t="s">
         <v>95</v>
       </c>
       <c r="H31" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="I31" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J31" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="K31" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="H34" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="I31" s="0" t="s">
+      <c r="I34" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="J31" s="0" t="s">
+      <c r="J34" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="K31" s="0" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="F32" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="G32" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="H32" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="I32" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="J32" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="K32" s="0" t="s">
+      <c r="K34" s="0" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1415,7 +1359,7 @@
         <v>107</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>13</v>
@@ -1424,132 +1368,114 @@
         <v>38</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="G35" s="0" t="s">
         <v>95</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="K35" s="0" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="B36" s="0" t="s">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="H38" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="C36" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E36" s="0" t="s">
+      <c r="I38" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="F36" s="0" t="s">
+      <c r="J38" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="G36" s="0" t="s">
+      <c r="K38" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G41" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="H36" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="I36" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="J36" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="K36" s="0" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="B39" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="E39" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="F39" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="G39" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="H39" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="I39" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="J39" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="K39" s="0" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="B42" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="E42" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="F42" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G42" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="H42" s="0" t="s">
+      <c r="H41" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="I42" s="0" t="s">
+      <c r="I41" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="J42" s="0" t="s">
+      <c r="J41" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="K42" s="0" t="s">
+      <c r="K41" s="0" t="s">
         <v>20</v>
       </c>
     </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Add the CF3hr & Esubhr reffclws combinations of this pextra variable to the missing identified list for pextra enabled #564.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables-enable-pextra.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables-enable-pextra.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="134">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -468,6 +468,18 @@
   </si>
   <si>
     <t xml:space="preserve">longitude latitude time typeli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CF3hr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reffclws</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From the AerChem side there is interest in Emon reffclws. This variable is identified as the already available PEXTRA variable with the table 126 grib code 126021, i.e. proposing to add reffclws as 21.126 to ifspar.json.  Note that this variable is not requested by CMIP6 AerChem, and that reffclws not occurs in any CMIP6 data request of the experiments in which any EC-Earth3* configuration participates. See further #564.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esubhr</t>
   </si>
 </sst>
 </file>
@@ -558,13 +570,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -647,7 +663,7 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="A44" activeCellId="0" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1465,6 +1481,35 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H44" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="I44" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H45" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="I45" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Update the pextra variant of the identified missing list #626.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables-enable-pextra.xlsx
+++ b/ece2cmor3/resources/list-of-identified-missing-cmpi6-requested-variables-enable-pextra.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="133">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -477,9 +477,6 @@
   </si>
   <si>
     <t xml:space="preserve">From the AerChem side there is interest in Emon reffclws. This variable is identified as the already available PEXTRA variable with the table 126 grib code 126021, i.e. proposing to add reffclws as 21.126 to ifspar.json.  Note that this variable is not requested by CMIP6 AerChem, and that reffclws not occurs in any CMIP6 data request of the experiments in which any EC-Earth3* configuration participates. See further #564.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Esubhr</t>
   </si>
 </sst>
 </file>
@@ -662,11 +659,11 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A44" activeCellId="0" sqref="A44"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
@@ -682,7 +679,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -717,7 +714,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>11</v>
       </c>
@@ -736,9 +733,9 @@
       <c r="F3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>17</v>
@@ -753,7 +750,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>21</v>
       </c>
@@ -772,9 +769,9 @@
       <c r="F5" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e9b495e2-5989-11e6-a4be-ac72891c3257.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>25</v>
@@ -789,7 +786,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>28</v>
       </c>
@@ -808,9 +805,9 @@
       <c r="F7" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/41455e80-4f40-11e6-a814-ac72891c3257.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H7" s="0" t="s">
         <v>33</v>
@@ -825,7 +822,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>36</v>
       </c>
@@ -844,9 +841,9 @@
       <c r="F9" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917acf0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H9" s="0" t="s">
         <v>41</v>
@@ -861,7 +858,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>36</v>
       </c>
@@ -880,9 +877,9 @@
       <c r="F10" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590de58a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H10" s="0" t="s">
         <v>48</v>
@@ -897,7 +894,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>36</v>
       </c>
@@ -916,9 +913,9 @@
       <c r="F11" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59147b48-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H11" s="0" t="s">
         <v>52</v>
@@ -933,7 +930,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>36</v>
       </c>
@@ -952,9 +949,9 @@
       <c r="F12" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="G12" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591444ca-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H12" s="0" t="s">
         <v>56</v>
@@ -969,7 +966,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>36</v>
       </c>
@@ -988,9 +985,9 @@
       <c r="F13" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="G13" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591720a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H13" s="0" t="s">
         <v>61</v>
@@ -1005,7 +1002,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>36</v>
       </c>
@@ -1024,9 +1021,9 @@
       <c r="F14" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="G14" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59177dc0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H14" s="0" t="s">
         <v>68</v>
@@ -1041,7 +1038,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>36</v>
       </c>
@@ -1060,9 +1057,9 @@
       <c r="F15" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="G15" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591306a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H15" s="0" t="s">
         <v>73</v>
@@ -1077,7 +1074,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>75</v>
       </c>
@@ -1096,9 +1093,9 @@
       <c r="F17" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="G17" s="0" t="n">
+      <c r="G17" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/9c35e2ac-a0de-11e6-bc63-ac72891c3257.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H17" s="0" t="s">
         <v>80</v>
@@ -1113,7 +1110,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>83</v>
       </c>
@@ -1132,9 +1129,9 @@
       <c r="F19" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G19" s="0" t="n">
+      <c r="G19" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H19" s="0" t="s">
         <v>86</v>
@@ -1149,7 +1146,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>83</v>
       </c>
@@ -1168,9 +1165,9 @@
       <c r="F20" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="0" t="n">
+      <c r="G20" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H20" s="0" t="s">
         <v>17</v>
@@ -1185,7 +1182,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>83</v>
       </c>
@@ -1204,9 +1201,9 @@
       <c r="F21" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G21" s="0" t="n">
+      <c r="G21" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/53826ae4-bf01-11e6-a554-ac72891c3257.html","web")</f>
-        <v>0</v>
+        <v>web</v>
       </c>
       <c r="H21" s="0" t="s">
         <v>90</v>
@@ -1221,13 +1218,6 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>92</v>
@@ -1333,8 +1323,6 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>107</v>
@@ -1405,8 +1393,6 @@
         <v>114</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>119</v>
@@ -1442,8 +1428,6 @@
         <v>127</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>128</v>
@@ -1479,8 +1463,6 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>130</v>
@@ -1495,21 +1477,6 @@
         <v>97</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="H45" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="I45" s="0" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>